<commit_message>
few errors fixed due to the updates on pom,
</commit_message>
<xml_diff>
--- a/src/test/java/Utilities/WriteInTheExcelFile.xlsx
+++ b/src/test/java/Utilities/WriteInTheExcelFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
   <si>
     <t>Merhaba Dünya</t>
   </si>
@@ -114,6 +114,54 @@
   </si>
   <si>
     <t>04_06_23171042</t>
+  </si>
+  <si>
+    <t>31_08_23125220</t>
+  </si>
+  <si>
+    <t>31_08_23125947</t>
+  </si>
+  <si>
+    <t>03_12_23194215</t>
+  </si>
+  <si>
+    <t>03_12_23200244</t>
+  </si>
+  <si>
+    <t>03_12_23201143</t>
+  </si>
+  <si>
+    <t>03_12_23204722</t>
+  </si>
+  <si>
+    <t>03_12_23204733</t>
+  </si>
+  <si>
+    <t>03_12_23204741</t>
+  </si>
+  <si>
+    <t>03_12_23204750</t>
+  </si>
+  <si>
+    <t>03_12_23204756</t>
+  </si>
+  <si>
+    <t>03_12_23211342</t>
+  </si>
+  <si>
+    <t>03_12_23213607</t>
+  </si>
+  <si>
+    <t>03_12_23214059</t>
+  </si>
+  <si>
+    <t>03_12_23214443</t>
+  </si>
+  <si>
+    <t>03_12_23215557</t>
+  </si>
+  <si>
+    <t>03_12_23215709</t>
   </si>
 </sst>
 </file>
@@ -432,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -696,6 +744,230 @@
         <v>29</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>